<commit_message>
edit sample names to match seqtab, required for script 08.phyloseq to perform correctly
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sequencing_Data_MiSeq\working_copies\251215_M06430_0030_000000000-M9JJFC\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sequencing_Data_MiSeq\working_copies\251215_M06430_0030_000000000-M9JJFC\SCAP_Faba_Fusarium_R_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD0FF77-B210-4CF0-9B10-F1F22B454F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CF4AEF-A447-4363-93BF-ACABA65D1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>sample</t>
   </si>
@@ -56,42 +56,6 @@
     <t>PCRnc</t>
   </si>
   <si>
-    <t>052_LB1</t>
-  </si>
-  <si>
-    <t>052_LB2</t>
-  </si>
-  <si>
-    <t>052_LB3</t>
-  </si>
-  <si>
-    <t>052_LB4</t>
-  </si>
-  <si>
-    <t>052_LB5</t>
-  </si>
-  <si>
-    <t>056_LB1</t>
-  </si>
-  <si>
-    <t>056_LB2</t>
-  </si>
-  <si>
-    <t>056_LB3</t>
-  </si>
-  <si>
-    <t>056_LB4</t>
-  </si>
-  <si>
-    <t>056_LB5</t>
-  </si>
-  <si>
-    <t>131_LB1</t>
-  </si>
-  <si>
-    <t>Xnc_LB1</t>
-  </si>
-  <si>
     <t>Faba052</t>
   </si>
   <si>
@@ -120,16 +84,64 @@
   </si>
   <si>
     <t>Faba</t>
+  </si>
+  <si>
+    <t>052-LB1_S14</t>
+  </si>
+  <si>
+    <t>052-LB2_S15</t>
+  </si>
+  <si>
+    <t>MC_S26_L001</t>
+  </si>
+  <si>
+    <t>PCRnc_S27_L</t>
+  </si>
+  <si>
+    <t>052-LB3_S16</t>
+  </si>
+  <si>
+    <t>052-LB4_S17</t>
+  </si>
+  <si>
+    <t>052-LB5_S18</t>
+  </si>
+  <si>
+    <t>056-LB1_S19</t>
+  </si>
+  <si>
+    <t>056-LB2_S20</t>
+  </si>
+  <si>
+    <t>056-LB3_S21</t>
+  </si>
+  <si>
+    <t>056-LB4_S22</t>
+  </si>
+  <si>
+    <t>056-LB5_S23</t>
+  </si>
+  <si>
+    <t>131-LB1_S24</t>
+  </si>
+  <si>
+    <t>Xnc-LB1_S25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -440,7 +452,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,205 +471,205 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>600</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>6000</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>60000</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>600000</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>600</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>6000</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>60000</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>600000</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -668,7 +680,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -682,7 +694,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -695,6 +707,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>